<commit_message>
Plot function and XLSX mapping update
New function for generating plots based on ggplot and updated mapping spreadsheet for correct identification of certain indicators.
</commit_message>
<xml_diff>
--- a/Plots/MDA_DataBook_mapping.xlsx
+++ b/Plots/MDA_DataBook_mapping.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldhealthorg-my.sharepoint.com/personal/bychkovs_who_int/Documents/Documents/STEPS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldhealthorg-my.sharepoint.com/personal/rakovaci_who_int/Documents/NCD (1)/STEPs/Country data/STEPS EURO data/STEPS EURO data anon/MDA_2021_STEPS/DataBook/Plots/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1091" documentId="8_{FC9006FC-0195-5042-A4D0-63813C14121B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9FEDF8BD-FD41-1D4B-B561-AC17144E1804}"/>
+  <xr:revisionPtr revIDLastSave="1141" documentId="8_{FC9006FC-0195-5042-A4D0-63813C14121B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81C66BE9-58F4-824B-9843-B3F905CEC10B}"/>
   <bookViews>
-    <workbookView xWindow="12260" yWindow="500" windowWidth="16540" windowHeight="16600" xr2:uid="{35027181-8D1F-4C47-B468-0C511EE20AD8}"/>
+    <workbookView xWindow="8860" yWindow="500" windowWidth="19940" windowHeight="16600" xr2:uid="{35027181-8D1F-4C47-B468-0C511EE20AD8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$192</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$195</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1249" uniqueCount="776">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1267" uniqueCount="784">
   <si>
     <t>script_name</t>
   </si>
@@ -2305,12 +2305,6 @@
     <t>1) Underweight &lt;18.5;2) Normal weight 18.5-24.9</t>
   </si>
   <si>
-    <t>1) blood glucose &lt;6.1;3) blood glucose &gt;=7.0 or took meds today</t>
-  </si>
-  <si>
-    <t>1) blood glucose &lt;6.1;2) blood glucose &gt;=6.1 AND &lt;7.0</t>
-  </si>
-  <si>
     <t>2) not currently on treatment for raised blood glucose;3) incomplete information regarding treatment for raised blood glucose</t>
   </si>
   <si>
@@ -2366,6 +2360,36 @@
   </si>
   <si>
     <t>2) not on medication</t>
+  </si>
+  <si>
+    <t>1) blood glucose &lt;6.1</t>
+  </si>
+  <si>
+    <t>pcomposition_work_list_long</t>
+  </si>
+  <si>
+    <t>pcomposition_trans_list_long</t>
+  </si>
+  <si>
+    <t>pcomposition_rec_list_long</t>
+  </si>
+  <si>
+    <t>pcomposition_rec</t>
+  </si>
+  <si>
+    <t>pcomposition_trans</t>
+  </si>
+  <si>
+    <t>pcomposition_work</t>
+  </si>
+  <si>
+    <t>Activity from work</t>
+  </si>
+  <si>
+    <t>Activity for transport</t>
+  </si>
+  <si>
+    <t>Activity during leisure time</t>
   </si>
 </sst>
 </file>
@@ -2381,12 +2405,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -2401,8 +2431,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2717,11 +2749,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{683DBB0C-090F-B94F-B48C-D3FDF1FE3576}">
-  <dimension ref="A1:I192"/>
+  <dimension ref="A1:I195"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A54" sqref="A54"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A97" sqref="A97:H99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3151,8 +3183,8 @@
       <c r="G16" t="s">
         <v>313</v>
       </c>
-      <c r="H16">
-        <v>1</v>
+      <c r="H16" s="1">
+        <v>7</v>
       </c>
       <c r="I16" t="s">
         <v>722</v>
@@ -3180,8 +3212,8 @@
       <c r="G17" t="s">
         <v>313</v>
       </c>
-      <c r="H17">
-        <v>1</v>
+      <c r="H17" s="1">
+        <v>7</v>
       </c>
       <c r="I17" t="s">
         <v>723</v>
@@ -4679,8 +4711,8 @@
       <c r="G72" t="s">
         <v>313</v>
       </c>
-      <c r="H72">
-        <v>1</v>
+      <c r="H72" s="1">
+        <v>3</v>
       </c>
       <c r="I72" t="s">
         <v>721</v>
@@ -5318,8 +5350,8 @@
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A96" t="b">
-        <v>1</v>
+      <c r="A96" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="B96" t="s">
         <v>135</v>
@@ -5344,83 +5376,80 @@
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A97" t="b">
-        <v>1</v>
-      </c>
-      <c r="B97" t="s">
+      <c r="A97" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B97" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C97" t="s">
-        <v>157</v>
-      </c>
-      <c r="D97" t="s">
-        <v>410</v>
-      </c>
-      <c r="E97" t="s">
-        <v>602</v>
-      </c>
-      <c r="F97" t="s">
-        <v>156</v>
-      </c>
-      <c r="G97" t="s">
-        <v>313</v>
-      </c>
-      <c r="H97">
-        <v>1</v>
-      </c>
-      <c r="I97" t="s">
-        <v>734</v>
+      <c r="C97" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>780</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="H97" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A98" t="b">
-        <v>1</v>
-      </c>
-      <c r="B98" t="s">
+      <c r="A98" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B98" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C98" t="s">
-        <v>159</v>
-      </c>
-      <c r="D98" t="s">
-        <v>411</v>
-      </c>
-      <c r="E98" t="s">
-        <v>603</v>
-      </c>
-      <c r="F98" t="s">
-        <v>158</v>
-      </c>
-      <c r="G98" t="s">
-        <v>314</v>
-      </c>
-      <c r="H98">
+      <c r="C98" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>776</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>779</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="H98" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A99" t="b">
-        <v>1</v>
-      </c>
-      <c r="B99" t="s">
+      <c r="A99" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B99" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C99" t="s">
-        <v>159</v>
-      </c>
-      <c r="D99" t="s">
-        <v>412</v>
-      </c>
-      <c r="E99" t="s">
-        <v>604</v>
-      </c>
-      <c r="F99" t="s">
-        <v>158</v>
-      </c>
-      <c r="G99" t="s">
-        <v>317</v>
-      </c>
-      <c r="H99">
+      <c r="C99" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>777</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>778</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>783</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="H99" s="1">
         <v>1</v>
       </c>
     </row>
@@ -5429,25 +5458,28 @@
         <v>1</v>
       </c>
       <c r="B100" t="s">
-        <v>160</v>
+        <v>135</v>
       </c>
       <c r="C100" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="D100" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="E100" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="F100" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="G100" t="s">
         <v>313</v>
       </c>
       <c r="H100">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="I100" t="s">
+        <v>734</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.2">
@@ -5455,28 +5487,25 @@
         <v>1</v>
       </c>
       <c r="B101" t="s">
-        <v>160</v>
+        <v>135</v>
       </c>
       <c r="C101" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D101" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="E101" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="F101" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="G101" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="H101">
         <v>1</v>
-      </c>
-      <c r="I101" t="s">
-        <v>735</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.2">
@@ -5484,28 +5513,25 @@
         <v>1</v>
       </c>
       <c r="B102" t="s">
-        <v>160</v>
+        <v>135</v>
       </c>
       <c r="C102" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="D102" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="E102" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="F102" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="G102" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="H102">
         <v>1</v>
-      </c>
-      <c r="I102" t="s">
-        <v>736</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.2">
@@ -5516,25 +5542,22 @@
         <v>160</v>
       </c>
       <c r="C103" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D103" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="E103" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="F103" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="G103" t="s">
         <v>313</v>
       </c>
       <c r="H103">
-        <v>1</v>
-      </c>
-      <c r="I103" t="s">
-        <v>737</v>
+        <v>4</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.2">
@@ -5542,25 +5565,28 @@
         <v>1</v>
       </c>
       <c r="B104" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C104" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="D104" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="E104" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="F104" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="G104" t="s">
         <v>313</v>
       </c>
       <c r="H104">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="I104" t="s">
+        <v>735</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.2">
@@ -5568,19 +5594,19 @@
         <v>1</v>
       </c>
       <c r="B105" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C105" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D105" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="E105" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="F105" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="G105" t="s">
         <v>313</v>
@@ -5589,7 +5615,7 @@
         <v>1</v>
       </c>
       <c r="I105" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.2">
@@ -5597,19 +5623,19 @@
         <v>1</v>
       </c>
       <c r="B106" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C106" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D106" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="E106" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="F106" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="G106" t="s">
         <v>313</v>
@@ -5618,7 +5644,7 @@
         <v>1</v>
       </c>
       <c r="I106" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.2">
@@ -5629,25 +5655,22 @@
         <v>167</v>
       </c>
       <c r="C107" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="D107" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="E107" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="F107" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="G107" t="s">
         <v>313</v>
       </c>
       <c r="H107">
-        <v>1</v>
-      </c>
-      <c r="I107" t="s">
-        <v>736</v>
+        <v>4</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.2">
@@ -5658,16 +5681,16 @@
         <v>167</v>
       </c>
       <c r="C108" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="D108" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="E108" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="F108" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G108" t="s">
         <v>313</v>
@@ -5676,7 +5699,7 @@
         <v>1</v>
       </c>
       <c r="I108" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
@@ -5684,25 +5707,28 @@
         <v>1</v>
       </c>
       <c r="B109" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="C109" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="D109" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="E109" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="F109" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="G109" t="s">
         <v>313</v>
       </c>
       <c r="H109">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="I109" t="s">
+        <v>738</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.2">
@@ -5710,19 +5736,19 @@
         <v>1</v>
       </c>
       <c r="B110" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="C110" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D110" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="E110" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="F110" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="G110" t="s">
         <v>313</v>
@@ -5731,7 +5757,7 @@
         <v>1</v>
       </c>
       <c r="I110" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.2">
@@ -5739,19 +5765,19 @@
         <v>1</v>
       </c>
       <c r="B111" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="C111" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="D111" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="E111" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="F111" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="G111" t="s">
         <v>313</v>
@@ -5760,7 +5786,7 @@
         <v>1</v>
       </c>
       <c r="I111" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.2">
@@ -5771,25 +5797,22 @@
         <v>175</v>
       </c>
       <c r="C112" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D112" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="E112" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="F112" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="G112" t="s">
         <v>313</v>
       </c>
       <c r="H112">
-        <v>1</v>
-      </c>
-      <c r="I112" t="s">
-        <v>737</v>
+        <v>4</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.2">
@@ -5797,19 +5820,19 @@
         <v>1</v>
       </c>
       <c r="B113" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="C113" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="D113" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="E113" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="F113" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="G113" t="s">
         <v>313</v>
@@ -5818,7 +5841,7 @@
         <v>1</v>
       </c>
       <c r="I113" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.2">
@@ -5826,19 +5849,19 @@
         <v>1</v>
       </c>
       <c r="B114" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="C114" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="D114" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="E114" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="F114" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="G114" t="s">
         <v>313</v>
@@ -5847,7 +5870,7 @@
         <v>1</v>
       </c>
       <c r="I114" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.2">
@@ -5855,19 +5878,19 @@
         <v>1</v>
       </c>
       <c r="B115" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="C115" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="D115" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="E115" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="F115" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="G115" t="s">
         <v>313</v>
@@ -5876,7 +5899,7 @@
         <v>1</v>
       </c>
       <c r="I115" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.2">
@@ -5887,16 +5910,16 @@
         <v>183</v>
       </c>
       <c r="C116" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D116" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="E116" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="F116" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="G116" t="s">
         <v>313</v>
@@ -5905,7 +5928,7 @@
         <v>1</v>
       </c>
       <c r="I116" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.2">
@@ -5919,13 +5942,13 @@
         <v>188</v>
       </c>
       <c r="D117" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="E117" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="F117" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="G117" t="s">
         <v>313</v>
@@ -5934,7 +5957,7 @@
         <v>1</v>
       </c>
       <c r="I117" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.2">
@@ -5942,19 +5965,19 @@
         <v>1</v>
       </c>
       <c r="B118" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="C118" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="D118" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="E118" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="F118" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="G118" t="s">
         <v>313</v>
@@ -5963,7 +5986,7 @@
         <v>1</v>
       </c>
       <c r="I118" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.2">
@@ -5971,19 +5994,19 @@
         <v>1</v>
       </c>
       <c r="B119" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="C119" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="D119" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="E119" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="F119" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="G119" t="s">
         <v>313</v>
@@ -5992,7 +6015,7 @@
         <v>1</v>
       </c>
       <c r="I119" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.2">
@@ -6000,19 +6023,19 @@
         <v>1</v>
       </c>
       <c r="B120" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="C120" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="D120" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="E120" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="F120" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="G120" t="s">
         <v>313</v>
@@ -6021,7 +6044,7 @@
         <v>1</v>
       </c>
       <c r="I120" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.2">
@@ -6035,13 +6058,13 @@
         <v>199</v>
       </c>
       <c r="D121" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="E121" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="F121" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G121" t="s">
         <v>313</v>
@@ -6050,7 +6073,7 @@
         <v>1</v>
       </c>
       <c r="I121" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.2">
@@ -6064,13 +6087,13 @@
         <v>199</v>
       </c>
       <c r="D122" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="E122" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="F122" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G122" t="s">
         <v>313</v>
@@ -6079,7 +6102,7 @@
         <v>1</v>
       </c>
       <c r="I122" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.2">
@@ -6093,13 +6116,13 @@
         <v>199</v>
       </c>
       <c r="D123" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="E123" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="F123" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G123" t="s">
         <v>313</v>
@@ -6108,7 +6131,7 @@
         <v>1</v>
       </c>
       <c r="I123" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.2">
@@ -6122,13 +6145,13 @@
         <v>199</v>
       </c>
       <c r="D124" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="E124" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="F124" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="G124" t="s">
         <v>313</v>
@@ -6137,7 +6160,7 @@
         <v>1</v>
       </c>
       <c r="I124" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.2">
@@ -6145,19 +6168,19 @@
         <v>1</v>
       </c>
       <c r="B125" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="C125" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D125" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="E125" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="F125" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="G125" t="s">
         <v>313</v>
@@ -6166,7 +6189,7 @@
         <v>1</v>
       </c>
       <c r="I125" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.2">
@@ -6174,19 +6197,19 @@
         <v>1</v>
       </c>
       <c r="B126" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="C126" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D126" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="E126" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="F126" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="G126" t="s">
         <v>313</v>
@@ -6195,7 +6218,7 @@
         <v>1</v>
       </c>
       <c r="I126" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.2">
@@ -6203,25 +6226,28 @@
         <v>1</v>
       </c>
       <c r="B127" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="C127" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="D127" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="E127" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="F127" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="G127" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H127">
         <v>1</v>
+      </c>
+      <c r="I127" t="s">
+        <v>748</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.2">
@@ -6229,25 +6255,28 @@
         <v>1</v>
       </c>
       <c r="B128" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C128" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D128" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="E128" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="F128" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="G128" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H128">
         <v>1</v>
+      </c>
+      <c r="I128" t="s">
+        <v>749</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.2">
@@ -6255,19 +6284,19 @@
         <v>1</v>
       </c>
       <c r="B129" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C129" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="D129" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="E129" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="F129" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="G129" t="s">
         <v>313</v>
@@ -6276,7 +6305,7 @@
         <v>1</v>
       </c>
       <c r="I129" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.2">
@@ -6287,25 +6316,22 @@
         <v>204</v>
       </c>
       <c r="C130" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D130" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="E130" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="F130" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="G130" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="H130">
         <v>1</v>
-      </c>
-      <c r="I130" t="s">
-        <v>751</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.2">
@@ -6316,25 +6342,22 @@
         <v>204</v>
       </c>
       <c r="C131" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D131" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="E131" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="F131" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="G131" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="H131">
         <v>1</v>
-      </c>
-      <c r="I131" t="s">
-        <v>752</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.2">
@@ -6348,13 +6371,13 @@
         <v>212</v>
       </c>
       <c r="D132" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="E132" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="F132" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G132" t="s">
         <v>313</v>
@@ -6363,7 +6386,7 @@
         <v>1</v>
       </c>
       <c r="I132" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.2">
@@ -6377,19 +6400,22 @@
         <v>212</v>
       </c>
       <c r="D133" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="E133" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="F133" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="G133" t="s">
         <v>313</v>
       </c>
       <c r="H133">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="I133" t="s">
+        <v>751</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.2">
@@ -6400,22 +6426,25 @@
         <v>204</v>
       </c>
       <c r="C134" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D134" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="E134" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="F134" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G134" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H134">
         <v>1</v>
+      </c>
+      <c r="I134" t="s">
+        <v>752</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.2">
@@ -6426,22 +6455,25 @@
         <v>204</v>
       </c>
       <c r="C135" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="D135" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="E135" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="F135" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="G135" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H135">
         <v>1</v>
+      </c>
+      <c r="I135" t="s">
+        <v>753</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.2">
@@ -6452,22 +6484,22 @@
         <v>204</v>
       </c>
       <c r="C136" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="D136" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="E136" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="F136" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="G136" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H136">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.2">
@@ -6478,16 +6510,16 @@
         <v>204</v>
       </c>
       <c r="C137" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D137" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="E137" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="F137" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="G137" t="s">
         <v>314</v>
@@ -6504,22 +6536,22 @@
         <v>204</v>
       </c>
       <c r="C138" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D138" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="E138" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="F138" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G138" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="H138">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.2">
@@ -6530,25 +6562,22 @@
         <v>204</v>
       </c>
       <c r="C139" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D139" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="E139" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="F139" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="G139" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="H139">
         <v>1</v>
-      </c>
-      <c r="I139" t="s">
-        <v>754</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.2">
@@ -6559,16 +6588,16 @@
         <v>204</v>
       </c>
       <c r="C140" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="D140" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="E140" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="F140" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="G140" t="s">
         <v>314</v>
@@ -6582,25 +6611,25 @@
         <v>1</v>
       </c>
       <c r="B141" t="s">
-        <v>225</v>
+        <v>204</v>
       </c>
       <c r="C141" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="D141" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="E141" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="F141" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="G141" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H141">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.2">
@@ -6608,25 +6637,28 @@
         <v>1</v>
       </c>
       <c r="B142" t="s">
-        <v>225</v>
+        <v>204</v>
       </c>
       <c r="C142" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="D142" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="E142" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="F142" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="G142" t="s">
-        <v>314</v>
-      </c>
-      <c r="H142">
-        <v>1</v>
+        <v>313</v>
+      </c>
+      <c r="H142" s="2">
+        <v>1</v>
+      </c>
+      <c r="I142" t="s">
+        <v>754</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.2">
@@ -6634,28 +6666,25 @@
         <v>1</v>
       </c>
       <c r="B143" t="s">
-        <v>225</v>
+        <v>204</v>
       </c>
       <c r="C143" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D143" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="E143" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="F143" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="G143" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="H143">
         <v>1</v>
-      </c>
-      <c r="I143" t="s">
-        <v>755</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.2">
@@ -6669,22 +6698,19 @@
         <v>228</v>
       </c>
       <c r="D144" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="E144" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="F144" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="G144" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="H144">
         <v>1</v>
-      </c>
-      <c r="I144" t="s">
-        <v>756</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.2">
@@ -6698,22 +6724,19 @@
         <v>228</v>
       </c>
       <c r="D145" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="E145" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="F145" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="G145" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="H145">
         <v>1</v>
-      </c>
-      <c r="I145" t="s">
-        <v>757</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.2">
@@ -6727,22 +6750,22 @@
         <v>228</v>
       </c>
       <c r="D146" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="E146" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="F146" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="G146" t="s">
         <v>313</v>
       </c>
-      <c r="H146">
-        <v>3</v>
+      <c r="H146" s="1">
+        <v>2</v>
       </c>
       <c r="I146" t="s">
-        <v>758</v>
+        <v>774</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.2">
@@ -6753,22 +6776,25 @@
         <v>225</v>
       </c>
       <c r="C147" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="D147" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="E147" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="F147" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="G147" t="s">
-        <v>314</v>
-      </c>
-      <c r="H147">
-        <v>1</v>
+        <v>313</v>
+      </c>
+      <c r="H147" s="1">
+        <v>2</v>
+      </c>
+      <c r="I147" t="s">
+        <v>774</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.2">
@@ -6779,22 +6805,25 @@
         <v>225</v>
       </c>
       <c r="C148" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="D148" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="E148" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="F148" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G148" t="s">
-        <v>314</v>
-      </c>
-      <c r="H148">
-        <v>1</v>
+        <v>313</v>
+      </c>
+      <c r="H148" s="2">
+        <v>1</v>
+      </c>
+      <c r="I148" t="s">
+        <v>755</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.2">
@@ -6805,25 +6834,25 @@
         <v>225</v>
       </c>
       <c r="C149" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="D149" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="E149" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="F149" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="G149" t="s">
         <v>313</v>
       </c>
       <c r="H149">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I149" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.2">
@@ -6837,22 +6866,19 @@
         <v>235</v>
       </c>
       <c r="D150" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="E150" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="F150" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="G150" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="H150">
         <v>1</v>
-      </c>
-      <c r="I150" t="s">
-        <v>760</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.2">
@@ -6866,22 +6892,19 @@
         <v>235</v>
       </c>
       <c r="D151" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="E151" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="F151" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="G151" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="H151">
         <v>1</v>
-      </c>
-      <c r="I151" t="s">
-        <v>759</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.2">
@@ -6895,13 +6918,13 @@
         <v>235</v>
       </c>
       <c r="D152" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="E152" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="F152" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="G152" t="s">
         <v>313</v>
@@ -6910,7 +6933,7 @@
         <v>1</v>
       </c>
       <c r="I152" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.2">
@@ -6918,19 +6941,19 @@
         <v>1</v>
       </c>
       <c r="B153" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="C153" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="D153" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="E153" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="F153" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="G153" t="s">
         <v>313</v>
@@ -6939,7 +6962,7 @@
         <v>1</v>
       </c>
       <c r="I153" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.2">
@@ -6947,19 +6970,19 @@
         <v>1</v>
       </c>
       <c r="B154" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="C154" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="D154" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="E154" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="F154" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="G154" t="s">
         <v>313</v>
@@ -6968,7 +6991,7 @@
         <v>1</v>
       </c>
       <c r="I154" t="s">
-        <v>762</v>
+        <v>757</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.2">
@@ -6976,25 +6999,28 @@
         <v>1</v>
       </c>
       <c r="B155" t="s">
-        <v>244</v>
+        <v>225</v>
       </c>
       <c r="C155" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="D155" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="E155" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="F155" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="G155" t="s">
         <v>313</v>
       </c>
       <c r="H155">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="I155" t="s">
+        <v>758</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.2">
@@ -7002,25 +7028,28 @@
         <v>1</v>
       </c>
       <c r="B156" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="C156" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="D156" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="E156" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="F156" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="G156" t="s">
         <v>313</v>
       </c>
       <c r="H156">
         <v>1</v>
+      </c>
+      <c r="I156" t="s">
+        <v>759</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.2">
@@ -7028,25 +7057,28 @@
         <v>1</v>
       </c>
       <c r="B157" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="C157" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="D157" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="E157" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="F157" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="G157" t="s">
         <v>313</v>
       </c>
       <c r="H157">
         <v>1</v>
+      </c>
+      <c r="I157" t="s">
+        <v>760</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.2">
@@ -7054,25 +7086,25 @@
         <v>1</v>
       </c>
       <c r="B158" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C158" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="D158" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="E158" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="F158" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="G158" t="s">
         <v>313</v>
       </c>
       <c r="H158">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.2">
@@ -7083,16 +7115,16 @@
         <v>246</v>
       </c>
       <c r="C159" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="D159" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="E159" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="F159" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="G159" t="s">
         <v>313</v>
@@ -7109,16 +7141,16 @@
         <v>246</v>
       </c>
       <c r="C160" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="D160" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="E160" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="F160" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="G160" t="s">
         <v>313</v>
@@ -7127,7 +7159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A161" t="b">
         <v>1</v>
       </c>
@@ -7135,16 +7167,16 @@
         <v>246</v>
       </c>
       <c r="C161" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D161" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="E161" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="F161" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="G161" t="s">
         <v>313</v>
@@ -7153,7 +7185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A162" t="b">
         <v>1</v>
       </c>
@@ -7161,25 +7193,25 @@
         <v>246</v>
       </c>
       <c r="C162" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="D162" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="E162" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="F162" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="G162" t="s">
         <v>313</v>
       </c>
       <c r="H162">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A163" t="b">
         <v>1</v>
       </c>
@@ -7187,16 +7219,16 @@
         <v>246</v>
       </c>
       <c r="C163" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="D163" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="E163" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="F163" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="G163" t="s">
         <v>313</v>
@@ -7205,7 +7237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A164" t="b">
         <v>1</v>
       </c>
@@ -7213,25 +7245,25 @@
         <v>246</v>
       </c>
       <c r="C164" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="D164" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="E164" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="F164" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="G164" t="s">
         <v>313</v>
       </c>
       <c r="H164">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A165" t="b">
         <v>1</v>
       </c>
@@ -7239,16 +7271,16 @@
         <v>246</v>
       </c>
       <c r="C165" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="D165" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="E165" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="F165" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="G165" t="s">
         <v>313</v>
@@ -7257,7 +7289,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A166" t="b">
         <v>1</v>
       </c>
@@ -7265,25 +7297,25 @@
         <v>246</v>
       </c>
       <c r="C166" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="D166" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="E166" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="F166" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="G166" t="s">
         <v>313</v>
       </c>
       <c r="H166">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A167" t="b">
         <v>1</v>
       </c>
@@ -7291,25 +7323,25 @@
         <v>246</v>
       </c>
       <c r="C167" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="D167" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="E167" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="F167" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="G167" t="s">
         <v>313</v>
       </c>
       <c r="H167">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A168" t="b">
         <v>1</v>
       </c>
@@ -7317,25 +7349,25 @@
         <v>246</v>
       </c>
       <c r="C168" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D168" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="E168" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
       <c r="F168" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="G168" t="s">
         <v>313</v>
       </c>
       <c r="H168">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A169" t="b">
         <v>1</v>
       </c>
@@ -7343,25 +7375,25 @@
         <v>246</v>
       </c>
       <c r="C169" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="D169" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="E169" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="F169" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="G169" t="s">
         <v>313</v>
       </c>
       <c r="H169">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A170" t="b">
         <v>1</v>
       </c>
@@ -7369,16 +7401,16 @@
         <v>246</v>
       </c>
       <c r="C170" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="D170" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="E170" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="F170" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="G170" t="s">
         <v>313</v>
@@ -7387,7 +7419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A171" t="b">
         <v>1</v>
       </c>
@@ -7395,25 +7427,25 @@
         <v>246</v>
       </c>
       <c r="C171" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="D171" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="E171" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="F171" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="G171" t="s">
         <v>313</v>
       </c>
       <c r="H171">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A172" t="b">
         <v>1</v>
       </c>
@@ -7421,25 +7453,25 @@
         <v>246</v>
       </c>
       <c r="C172" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="D172" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="E172" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="F172" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="G172" t="s">
         <v>313</v>
       </c>
       <c r="H172">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A173" t="b">
         <v>1</v>
       </c>
@@ -7447,25 +7479,25 @@
         <v>246</v>
       </c>
       <c r="C173" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="D173" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="E173" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="F173" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="G173" t="s">
         <v>313</v>
       </c>
       <c r="H173">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A174" t="b">
         <v>1</v>
       </c>
@@ -7473,16 +7505,16 @@
         <v>246</v>
       </c>
       <c r="C174" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="D174" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="E174" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="F174" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="G174" t="s">
         <v>313</v>
@@ -7491,7 +7523,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A175" t="b">
         <v>1</v>
       </c>
@@ -7499,51 +7531,48 @@
         <v>246</v>
       </c>
       <c r="C175" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="D175" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="E175" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="F175" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="G175" t="s">
         <v>313</v>
       </c>
       <c r="H175">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A176" t="b">
         <v>1</v>
       </c>
       <c r="B176" t="s">
-        <v>286</v>
+        <v>246</v>
       </c>
       <c r="C176" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="D176" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="E176" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="F176" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="G176" t="s">
         <v>313</v>
       </c>
       <c r="H176">
-        <v>1</v>
-      </c>
-      <c r="I176" t="s">
-        <v>763</v>
+        <v>4</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.2">
@@ -7551,28 +7580,25 @@
         <v>1</v>
       </c>
       <c r="B177" t="s">
-        <v>286</v>
+        <v>246</v>
       </c>
       <c r="C177" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="D177" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="E177" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="F177" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="G177" t="s">
         <v>313</v>
       </c>
       <c r="H177">
-        <v>1</v>
-      </c>
-      <c r="I177" t="s">
-        <v>763</v>
+        <v>4</v>
       </c>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.2">
@@ -7580,28 +7606,25 @@
         <v>1</v>
       </c>
       <c r="B178" t="s">
-        <v>286</v>
+        <v>246</v>
       </c>
       <c r="C178" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="D178" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="E178" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="F178" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="G178" t="s">
         <v>313</v>
       </c>
       <c r="H178">
-        <v>1</v>
-      </c>
-      <c r="I178" t="s">
-        <v>764</v>
+        <v>5</v>
       </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.2">
@@ -7612,16 +7635,16 @@
         <v>286</v>
       </c>
       <c r="C179" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="D179" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="E179" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="F179" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="G179" t="s">
         <v>313</v>
@@ -7630,7 +7653,7 @@
         <v>1</v>
       </c>
       <c r="I179" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.2">
@@ -7641,16 +7664,16 @@
         <v>286</v>
       </c>
       <c r="C180" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="D180" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="E180" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
       <c r="F180" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="G180" t="s">
         <v>313</v>
@@ -7659,7 +7682,7 @@
         <v>1</v>
       </c>
       <c r="I180" t="s">
-        <v>766</v>
+        <v>761</v>
       </c>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.2">
@@ -7670,16 +7693,16 @@
         <v>286</v>
       </c>
       <c r="C181" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D181" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="E181" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="F181" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="G181" t="s">
         <v>313</v>
@@ -7688,7 +7711,7 @@
         <v>1</v>
       </c>
       <c r="I181" t="s">
-        <v>767</v>
+        <v>762</v>
       </c>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.2">
@@ -7699,22 +7722,25 @@
         <v>286</v>
       </c>
       <c r="C182" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="D182" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="E182" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="F182" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="G182" t="s">
         <v>313</v>
       </c>
       <c r="H182">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="I182" t="s">
+        <v>763</v>
       </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.2">
@@ -7725,16 +7751,16 @@
         <v>286</v>
       </c>
       <c r="C183" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="D183" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="E183" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
       <c r="F183" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="G183" t="s">
         <v>313</v>
@@ -7743,7 +7769,7 @@
         <v>1</v>
       </c>
       <c r="I183" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.2">
@@ -7754,16 +7780,16 @@
         <v>286</v>
       </c>
       <c r="C184" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="D184" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="E184" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="F184" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="G184" t="s">
         <v>313</v>
@@ -7772,7 +7798,7 @@
         <v>1</v>
       </c>
       <c r="I184" t="s">
-        <v>769</v>
+        <v>765</v>
       </c>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.2">
@@ -7783,25 +7809,22 @@
         <v>286</v>
       </c>
       <c r="C185" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="D185" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="E185" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
       <c r="F185" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="G185" t="s">
         <v>313</v>
       </c>
       <c r="H185">
-        <v>1</v>
-      </c>
-      <c r="I185" t="s">
-        <v>770</v>
+        <v>5</v>
       </c>
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.2">
@@ -7812,16 +7835,16 @@
         <v>286</v>
       </c>
       <c r="C186" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D186" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="E186" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="F186" t="s">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="G186" t="s">
         <v>313</v>
@@ -7830,7 +7853,7 @@
         <v>1</v>
       </c>
       <c r="I186" t="s">
-        <v>771</v>
+        <v>766</v>
       </c>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.2">
@@ -7841,16 +7864,16 @@
         <v>286</v>
       </c>
       <c r="C187" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D187" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="E187" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="F187" t="s">
-        <v>502</v>
+        <v>301</v>
       </c>
       <c r="G187" t="s">
         <v>313</v>
@@ -7859,7 +7882,7 @@
         <v>1</v>
       </c>
       <c r="I187" t="s">
-        <v>772</v>
+        <v>767</v>
       </c>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.2">
@@ -7867,19 +7890,19 @@
         <v>1</v>
       </c>
       <c r="B188" t="s">
-        <v>306</v>
+        <v>286</v>
       </c>
       <c r="C188" t="s">
-        <v>503</v>
+        <v>304</v>
       </c>
       <c r="D188" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
       <c r="E188" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="F188" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="G188" t="s">
         <v>313</v>
@@ -7888,7 +7911,7 @@
         <v>1</v>
       </c>
       <c r="I188" t="s">
-        <v>773</v>
+        <v>768</v>
       </c>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.2">
@@ -7896,19 +7919,19 @@
         <v>1</v>
       </c>
       <c r="B189" t="s">
-        <v>306</v>
+        <v>286</v>
       </c>
       <c r="C189" t="s">
-        <v>503</v>
+        <v>305</v>
       </c>
       <c r="D189" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="E189" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="F189" t="s">
-        <v>308</v>
+        <v>500</v>
       </c>
       <c r="G189" t="s">
         <v>313</v>
@@ -7917,7 +7940,7 @@
         <v>1</v>
       </c>
       <c r="I189" t="s">
-        <v>774</v>
+        <v>769</v>
       </c>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.2">
@@ -7925,19 +7948,19 @@
         <v>1</v>
       </c>
       <c r="B190" t="s">
-        <v>306</v>
+        <v>286</v>
       </c>
       <c r="C190" t="s">
-        <v>503</v>
+        <v>305</v>
       </c>
       <c r="D190" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="E190" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="F190" t="s">
-        <v>309</v>
+        <v>502</v>
       </c>
       <c r="G190" t="s">
         <v>313</v>
@@ -7946,7 +7969,7 @@
         <v>1</v>
       </c>
       <c r="I190" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.2">
@@ -7960,13 +7983,13 @@
         <v>503</v>
       </c>
       <c r="D191" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="E191" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="F191" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="G191" t="s">
         <v>313</v>
@@ -7975,7 +7998,7 @@
         <v>1</v>
       </c>
       <c r="I191" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.2">
@@ -7989,26 +8012,113 @@
         <v>503</v>
       </c>
       <c r="D192" t="s">
+        <v>505</v>
+      </c>
+      <c r="E192" t="s">
+        <v>694</v>
+      </c>
+      <c r="F192" t="s">
+        <v>308</v>
+      </c>
+      <c r="G192" t="s">
+        <v>313</v>
+      </c>
+      <c r="H192">
+        <v>1</v>
+      </c>
+      <c r="I192" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A193" t="b">
+        <v>1</v>
+      </c>
+      <c r="B193" t="s">
+        <v>306</v>
+      </c>
+      <c r="C193" t="s">
+        <v>503</v>
+      </c>
+      <c r="D193" t="s">
+        <v>506</v>
+      </c>
+      <c r="E193" t="s">
+        <v>695</v>
+      </c>
+      <c r="F193" t="s">
+        <v>309</v>
+      </c>
+      <c r="G193" t="s">
+        <v>313</v>
+      </c>
+      <c r="H193">
+        <v>1</v>
+      </c>
+      <c r="I193" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A194" t="b">
+        <v>1</v>
+      </c>
+      <c r="B194" t="s">
+        <v>306</v>
+      </c>
+      <c r="C194" t="s">
+        <v>503</v>
+      </c>
+      <c r="D194" t="s">
+        <v>507</v>
+      </c>
+      <c r="E194" t="s">
+        <v>696</v>
+      </c>
+      <c r="F194" t="s">
+        <v>310</v>
+      </c>
+      <c r="G194" t="s">
+        <v>313</v>
+      </c>
+      <c r="H194">
+        <v>1</v>
+      </c>
+      <c r="I194" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A195" t="b">
+        <v>1</v>
+      </c>
+      <c r="B195" t="s">
+        <v>306</v>
+      </c>
+      <c r="C195" t="s">
+        <v>503</v>
+      </c>
+      <c r="D195" t="s">
         <v>508</v>
       </c>
-      <c r="E192" t="s">
+      <c r="E195" t="s">
         <v>697</v>
       </c>
-      <c r="F192" t="s">
+      <c r="F195" t="s">
         <v>311</v>
       </c>
-      <c r="G192" t="s">
-        <v>313</v>
-      </c>
-      <c r="H192">
-        <v>1</v>
-      </c>
-      <c r="I192" t="s">
-        <v>775</v>
+      <c r="G195" t="s">
+        <v>313</v>
+      </c>
+      <c r="H195">
+        <v>1</v>
+      </c>
+      <c r="I195" t="s">
+        <v>773</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I192" xr:uid="{683DBB0C-090F-B94F-B48C-D3FDF1FE3576}"/>
+  <autoFilter ref="A1:I195" xr:uid="{683DBB0C-090F-B94F-B48C-D3FDF1FE3576}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>